<commit_message>
Payments Update UPdate 5/13/2025
</commit_message>
<xml_diff>
--- a/Payment Data Base.xlsx
+++ b/Payment Data Base.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr hidePivotFieldList="1"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Input Sheet" sheetId="4" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="80">
   <si>
     <t>Payment Record</t>
   </si>
@@ -91,13 +91,22 @@
     <t>February</t>
   </si>
   <si>
+    <t>Jenelyn Madriaga</t>
+  </si>
+  <si>
     <t>Anie Lagrimas</t>
+  </si>
+  <si>
+    <t>Dennis Padilla</t>
   </si>
   <si>
     <t>April Rose Mayo</t>
   </si>
   <si>
     <t>April</t>
+  </si>
+  <si>
+    <t>Nathaniel Guevarra Aguilar</t>
   </si>
   <si>
     <t>Arlene Lobo Paule</t>
@@ -116,9 +125,6 @@
   </si>
   <si>
     <t>July</t>
-  </si>
-  <si>
-    <t>Dennis Padilla</t>
   </si>
   <si>
     <t>August</t>
@@ -152,9 +158,6 @@
   </si>
   <si>
     <t>Jc Noah Belbar</t>
-  </si>
-  <si>
-    <t>Jenelyn Madriaga</t>
   </si>
   <si>
     <t>Jenelyn Cioco</t>
@@ -226,7 +229,58 @@
     <t>Ryan Austria</t>
   </si>
   <si>
-    <t>Sum of PAID AMOUNT</t>
+    <t>100 Total</t>
+  </si>
+  <si>
+    <t>23 Total</t>
+  </si>
+  <si>
+    <t>March Total</t>
+  </si>
+  <si>
+    <t>29 Total</t>
+  </si>
+  <si>
+    <t>April Total</t>
+  </si>
+  <si>
+    <t>2025 Total</t>
+  </si>
+  <si>
+    <t>Aubrey Cerezo Crespo Total</t>
+  </si>
+  <si>
+    <t>21 Total</t>
+  </si>
+  <si>
+    <t>28 Total</t>
+  </si>
+  <si>
+    <t>Charlie Timbalaco Total</t>
+  </si>
+  <si>
+    <t>22 Total</t>
+  </si>
+  <si>
+    <t>26 Total</t>
+  </si>
+  <si>
+    <t>Dennis Padilla Total</t>
+  </si>
+  <si>
+    <t>3 Total</t>
+  </si>
+  <si>
+    <t>19 Total</t>
+  </si>
+  <si>
+    <t>Jamaiza Campomayor Total</t>
+  </si>
+  <si>
+    <t>Jenelyn Madriaga Total</t>
+  </si>
+  <si>
+    <t>Nathaniel Guevarra Aguilar Total</t>
   </si>
   <si>
     <t>Grand Total</t>
@@ -1021,10 +1075,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1157,7 +1211,7 @@
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="87">
+  <dxfs count="71">
     <dxf>
       <alignment horizontal="center"/>
     </dxf>
@@ -1474,54 +1528,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="179" formatCode="mmmmm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="179" formatCode="mmmmm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="179" formatCode="mmmmm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="179" formatCode="mmmmm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="179" formatCode="mmmmm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="179" formatCode="mmmmm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="179" formatCode="mmmmm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="179" formatCode="mmmmm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="179" formatCode="mmmmm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="179" formatCode="mmmmm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="179" formatCode="mmmmm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="[$PHP]\ #,##0.00;[$PHP]\ \-#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="[$PHP]\ #,##0.00;[$PHP]\ \-#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="[$PHP]\ #,##0.00;[$PHP]\ \-#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="[$PHP]\ #,##0.00;[$PHP]\ \-#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="[$PHP]\ #,##0.00;[$PHP]\ \-#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="[$PHP]\ #,##0.00;[$PHP]\ \-#,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="178" formatCode="[$PHP]\ #,##0.00;[$PHP]\ \-#,##0.00"/>
@@ -1866,34 +1872,34 @@
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
     <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="69"/>
-      <tableStyleElement type="headerRow" dxfId="68"/>
-      <tableStyleElement type="totalRow" dxfId="67"/>
-      <tableStyleElement type="firstColumn" dxfId="66"/>
-      <tableStyleElement type="lastColumn" dxfId="65"/>
-      <tableStyleElement type="firstRowStripe" dxfId="64"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="63"/>
+      <tableStyleElement type="wholeTable" dxfId="53"/>
+      <tableStyleElement type="headerRow" dxfId="52"/>
+      <tableStyleElement type="totalRow" dxfId="51"/>
+      <tableStyleElement type="firstColumn" dxfId="50"/>
+      <tableStyleElement type="lastColumn" dxfId="49"/>
+      <tableStyleElement type="firstRowStripe" dxfId="48"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="47"/>
     </tableStyle>
     <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="79"/>
-      <tableStyleElement type="totalRow" dxfId="78"/>
-      <tableStyleElement type="firstRowStripe" dxfId="77"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="76"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="75"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="74"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="73"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="72"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="71"/>
-      <tableStyleElement type="pageFieldValues" dxfId="70"/>
+      <tableStyleElement type="headerRow" dxfId="63"/>
+      <tableStyleElement type="totalRow" dxfId="62"/>
+      <tableStyleElement type="firstRowStripe" dxfId="61"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="60"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="59"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="58"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="57"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="56"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="55"/>
+      <tableStyleElement type="pageFieldValues" dxfId="54"/>
     </tableStyle>
     <tableStyle name="PivotStylePreset6_Accent1" table="0" count="7" xr9:uid="{C14D74E0-0E90-48FA-A4CF-29A2662E7F7C}">
-      <tableStyleElement type="wholeTable" dxfId="86"/>
-      <tableStyleElement type="firstColumn" dxfId="85"/>
-      <tableStyleElement type="firstRowStripe" dxfId="84"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="83"/>
-      <tableStyleElement type="firstSubtotalColumn" dxfId="82"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="81"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="80"/>
+      <tableStyleElement type="wholeTable" dxfId="70"/>
+      <tableStyleElement type="firstColumn" dxfId="69"/>
+      <tableStyleElement type="firstRowStripe" dxfId="68"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="67"/>
+      <tableStyleElement type="firstSubtotalColumn" dxfId="66"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="65"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="64"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1918,7 +1924,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Reunion.xlsx]Sorting Sheet!PivotTable6</c:name>
+    <c:name>[Payment Data Base.xlsx]Sorting Sheet!PivotTable6</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -1927,155 +1933,18 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+        <c:grouping val="percentStacked"/>
         <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sorting Sheet'!$G$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="203200" dist="279400" dir="8100000" algn="tr" rotWithShape="0">
-                <a:prstClr val="black">
-                  <a:alpha val="40000"/>
-                </a:prstClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'Sorting Sheet'!$A$4:$F$6</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="1"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>G- Cash</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>3</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>March</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>2025</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>100</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Jamaiza Campomayor</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sorting Sheet'!$G$4:$G$6</c:f>
-              <c:numCache>
-                <c:formatCode>[$PHP]\ #,##0.00;[$PHP]\ \-#,##0.00</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="246"/>
-        <c:overlap val="-28"/>
+        <c:gapWidth val="500"/>
+        <c:overlap val="100"/>
         <c:axId val="567797464"/>
         <c:axId val="945219092"/>
       </c:barChart>
@@ -2093,7 +1962,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
+              <a:schemeClr val="dk1">
                 <a:lumMod val="15000"/>
                 <a:lumOff val="85000"/>
               </a:schemeClr>
@@ -2107,9 +1976,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -2148,7 +2017,37 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="[$PHP]\ #,##0.00;[$PHP]\ \-#,##0.00" sourceLinked="1"/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2164,9 +2063,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -2182,6 +2081,44 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2201,7 +2138,9 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="96000"/>
+      </a:schemeClr>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -2219,7 +2158,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr lang="en-US" sz="1000"/>
+        <a:defRPr lang="en-US"/>
       </a:pPr>
     </a:p>
   </c:txPr>
@@ -2281,13 +2220,13 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="10001">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="10027">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -2299,7 +2238,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -2307,7 +2246,7 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2326,7 +2265,9 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="96000"/>
+        </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -2345,7 +2286,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="75000"/>
         <a:lumOff val="25000"/>
       </a:schemeClr>
@@ -2384,7 +2325,7 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
@@ -2392,8 +2333,36 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:hueOff val="-1670000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
       <a:ln>
-        <a:noFill/>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="75000"/>
+                <a:hueOff val="-1670000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5280000" scaled="0"/>
+        </a:gradFill>
       </a:ln>
       <a:effectLst/>
     </cs:spPr>
@@ -2469,7 +2438,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -2478,7 +2447,7 @@
       <a:noFill/>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2493,22 +2462,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2520,14 +2490,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -2541,7 +2510,7 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -2609,14 +2578,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="75000"/>
             <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -2628,14 +2596,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -2644,7 +2611,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -2672,7 +2639,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -2687,14 +2654,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -2703,7 +2669,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="75000"/>
         <a:lumOff val="25000"/>
       </a:schemeClr>
@@ -2733,7 +2699,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -2745,19 +2711,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2766,7 +2733,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -2807,15 +2774,15 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="12" name="Group 11"/>
+        <xdr:cNvPr id="5" name="Group 4"/>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8895080" y="379095"/>
+          <a:off x="9608820" y="379095"/>
           <a:ext cx="5535295" cy="6365240"/>
           <a:chOff x="14015" y="574"/>
-          <a:chExt cx="8717" cy="3679"/>
+          <a:chExt cx="8717" cy="9832"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2827,7 +2794,7 @@
             </xdr:nvGraphicFramePr>
             <xdr:xfrm>
               <a:off x="14015" y="574"/>
-              <a:ext cx="2880" cy="3666"/>
+              <a:ext cx="2880" cy="9797"/>
             </xdr:xfrm>
             <a:graphic>
               <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
@@ -2847,7 +2814,7 @@
             <xdr:spPr>
               <a:xfrm>
                 <a:off x="14015" y="574"/>
-                <a:ext cx="2880" cy="3666"/>
+                <a:ext cx="2880" cy="9797"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
                 <a:avLst/>
@@ -2881,9 +2848,9 @@
           <xdr:cNvGrpSpPr/>
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="16938" y="583"/>
-            <a:ext cx="5794" cy="3670"/>
+          <a:xfrm rot="0">
+            <a:off x="16938" y="598"/>
+            <a:ext cx="5794" cy="9808"/>
             <a:chOff x="14015" y="542"/>
             <a:chExt cx="5794" cy="3670"/>
           </a:xfrm>
@@ -3045,20 +3012,22 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" refreshedDate="45719.651724537" refreshedBy="denni" recordCount="2">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" refreshedDate="45790.4240856481" refreshedBy="denni" recordCount="11">
   <cacheSource type="worksheet">
     <worksheetSource name="Table4"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="MEMBERS" numFmtId="0">
-      <sharedItems containsBlank="1" count="13">
+      <sharedItems containsBlank="1" count="15">
         <s v="Jamaiza Campomayor"/>
+        <s v="Jenelyn Madriaga"/>
+        <s v="Dennis Padilla"/>
+        <s v="Nathaniel Guevarra Aguilar"/>
+        <s v="Aubrey Cerezo Crespo"/>
+        <s v="Charlie Timbalaco"/>
         <m/>
-        <s v="Aubrey Cerezo Crespo" u="1"/>
         <s v="Arlene Lobo Paule" u="1"/>
-        <s v="Charlie Timbalaco" u="1"/>
         <s v="Dinzy Mae Doblin" u="1"/>
-        <s v="Dennis Padilla" u="1"/>
         <s v="Niever Owel" u="1"/>
         <s v="Quim Cadaa" u="1"/>
         <s v="Lusvin Ibanez Papuran" u="1"/>
@@ -3084,23 +3053,26 @@
     <cacheField name="Month" numFmtId="179">
       <sharedItems containsBlank="1" count="5">
         <s v="March"/>
+        <s v="April"/>
         <m/>
-        <s v="April" u="1"/>
         <s v="May" u="1"/>
         <s v="January" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Day" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="30" count="12">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="30" count="15">
         <n v="3"/>
+        <n v="21"/>
+        <n v="22"/>
+        <n v="23"/>
+        <n v="19"/>
+        <n v="26"/>
+        <n v="28"/>
+        <n v="29"/>
         <m/>
         <n v="30" u="1"/>
-        <n v="28" u="1"/>
-        <n v="29" u="1"/>
         <n v="20" u="1"/>
         <n v="25" u="1"/>
-        <n v="21" u="1"/>
-        <n v="26" u="1"/>
         <n v="1" u="1"/>
         <n v="2" u="1"/>
         <n v="5" u="1"/>
@@ -3126,7 +3098,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="2">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="11">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -3137,10 +3109,82 @@
   </r>
   <r>
     <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="2"/>
+    <x v="8"/>
     <x v="1"/>
   </r>
 </pivotCacheRecords>
@@ -3148,94 +3192,418 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="0" autoFormatId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" createdVersion="5" showMissing="0" useAutoFormatting="1" compact="0" indent="0" compactData="0" showDrill="0" multipleFieldFilters="0" fieldListSortAscending="1" chartFormat="6">
-  <location ref="A3:G6" firstHeaderRow="1" firstDataRow="1" firstDataCol="6"/>
+  <location ref="A3:F98" firstHeaderRow="1" firstDataRow="1" firstDataCol="6"/>
   <pivotFields count="6">
-    <pivotField axis="axisRow" compact="0" insertBlankRow="1" sortType="ascending" defaultSubtotal="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="13">
-        <item m="1" x="3"/>
-        <item m="1" x="2"/>
-        <item m="1" x="4"/>
-        <item m="1" x="6"/>
-        <item m="1" x="5"/>
+    <pivotField axis="axisRow" compact="0" insertBlankRow="1" sortType="ascending" outline="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="16">
+        <item m="1" x="7"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item m="1" x="8"/>
         <item x="0"/>
+        <item x="1"/>
+        <item m="1" x="11"/>
+        <item x="3"/>
         <item m="1" x="9"/>
-        <item m="1" x="7"/>
-        <item m="1" x="8"/>
         <item m="1" x="10"/>
-        <item m="1" x="11"/>
         <item m="1" x="12"/>
-        <item h="1" x="1"/>
+        <item m="1" x="13"/>
+        <item m="1" x="14"/>
+        <item h="1" x="6"/>
+        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" dataField="1" compact="0" insertBlankRow="1" sortType="ascending" defaultSubtotal="0" outline="0" showAll="0">
-      <items count="4">
+    <pivotField axis="axisRow" compact="0" insertBlankRow="1" sortType="ascending" outline="0" showAll="0">
+      <items count="5">
         <item x="0"/>
         <item m="1" x="2"/>
         <item m="1" x="3"/>
         <item x="1"/>
+        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" compact="0" insertBlankRow="1" sortType="ascending" defaultSubtotal="0" outline="0" showAll="0">
-      <items count="2">
+    <pivotField axis="axisRow" compact="0" insertBlankRow="1" sortType="ascending" outline="0" showAll="0">
+      <items count="3">
         <item x="0"/>
-        <item h="1" x="1"/>
+        <item x="1"/>
+        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" compact="0" insertBlankRow="1" sortType="ascending" defaultSubtotal="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
+    <pivotField axis="axisRow" compact="0" insertBlankRow="1" sortType="ascending" outline="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="6">
         <item m="1" x="4"/>
         <item x="0"/>
-        <item m="1" x="2"/>
+        <item x="1"/>
         <item m="1" x="3"/>
-        <item h="1" x="1"/>
+        <item x="2"/>
+        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" compact="0" insertBlankRow="1" sortType="ascending" defaultSubtotal="0" outline="0" showAll="0">
-      <items count="12">
+    <pivotField axis="axisRow" compact="0" insertBlankRow="1" sortType="ascending" outline="0" showAll="0">
+      <items count="16">
+        <item m="1" x="12"/>
+        <item m="1" x="13"/>
+        <item x="0"/>
+        <item m="1" x="14"/>
+        <item x="4"/>
+        <item m="1" x="10"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item m="1" x="11"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
         <item m="1" x="9"/>
-        <item m="1" x="10"/>
-        <item x="0"/>
-        <item m="1" x="11"/>
-        <item m="1" x="5"/>
-        <item m="1" x="7"/>
-        <item m="1" x="6"/>
-        <item m="1" x="8"/>
-        <item m="1" x="3"/>
-        <item m="1" x="4"/>
-        <item m="1" x="2"/>
-        <item x="1"/>
+        <item x="8"/>
+        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" compact="0" insertBlankRow="1" sortType="ascending" defaultSubtotal="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="6">
+    <pivotField axis="axisRow" compact="0" insertBlankRow="1" sortType="ascending" outline="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="7">
         <item m="1" x="5"/>
         <item m="1" x="4"/>
         <item m="1" x="2"/>
         <item x="0"/>
         <item m="1" x="3"/>
         <item x="1"/>
+        <item t="default"/>
       </items>
     </pivotField>
   </pivotFields>
   <rowFields count="6">
     <field x="0"/>
-    <field x="1"/>
     <field x="2"/>
     <field x="3"/>
     <field x="4"/>
+    <field x="1"/>
     <field x="5"/>
   </rowFields>
-  <rowItems count="3">
+  <rowItems count="95">
+    <i>
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+      <x v="8"/>
+      <x/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="4">
+      <x/>
+    </i>
+    <i t="blank" r="4">
+      <x/>
+    </i>
+    <i t="default" r="3">
+      <x v="8"/>
+    </i>
+    <i t="blank" r="3">
+      <x v="8"/>
+    </i>
+    <i t="default" r="2">
+      <x v="1"/>
+    </i>
+    <i t="blank" r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+      <x v="12"/>
+      <x/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="4">
+      <x/>
+    </i>
+    <i t="blank" r="4">
+      <x/>
+    </i>
+    <i t="default" r="3">
+      <x v="12"/>
+    </i>
+    <i t="blank" r="3">
+      <x v="12"/>
+    </i>
+    <i t="default" r="2">
+      <x v="2"/>
+    </i>
+    <i t="blank" r="2">
+      <x v="2"/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i t="blank" r="1">
+      <x/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i t="blank">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+      <x v="1"/>
+      <x v="6"/>
+      <x/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="4">
+      <x/>
+    </i>
+    <i t="blank" r="4">
+      <x/>
+    </i>
+    <i t="default" r="3">
+      <x v="6"/>
+    </i>
+    <i t="blank" r="3">
+      <x v="6"/>
+    </i>
+    <i t="default" r="2">
+      <x v="1"/>
+    </i>
+    <i t="blank" r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+      <x v="11"/>
+      <x/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="4">
+      <x/>
+    </i>
+    <i t="blank" r="4">
+      <x/>
+    </i>
+    <i t="default" r="3">
+      <x v="11"/>
+    </i>
+    <i t="blank" r="3">
+      <x v="11"/>
+    </i>
+    <i t="default" r="2">
+      <x v="2"/>
+    </i>
+    <i t="blank" r="2">
+      <x v="2"/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i t="blank" r="1">
+      <x/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="blank">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x/>
+      <x v="1"/>
+      <x v="7"/>
+      <x/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="4">
+      <x/>
+    </i>
+    <i t="blank" r="4">
+      <x/>
+    </i>
+    <i t="default" r="3">
+      <x v="7"/>
+    </i>
+    <i t="blank" r="3">
+      <x v="7"/>
+    </i>
+    <i t="default" r="2">
+      <x v="1"/>
+    </i>
+    <i t="blank" r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+      <x v="10"/>
+      <x/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="4">
+      <x/>
+    </i>
+    <i t="blank" r="4">
+      <x/>
+    </i>
+    <i t="default" r="3">
+      <x v="10"/>
+    </i>
+    <i t="blank" r="3">
+      <x v="10"/>
+    </i>
+    <i t="default" r="2">
+      <x v="2"/>
+    </i>
+    <i t="blank" r="2">
+      <x v="2"/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i t="blank" r="1">
+      <x/>
+    </i>
+    <i t="default">
+      <x v="3"/>
+    </i>
+    <i t="blank">
+      <x v="3"/>
+    </i>
     <i>
       <x v="5"/>
       <x/>
+      <x v="1"/>
+      <x v="2"/>
+      <x/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="4">
+      <x/>
+    </i>
+    <i t="blank" r="4">
+      <x/>
+    </i>
+    <i t="default" r="3">
+      <x v="2"/>
+    </i>
+    <i t="blank" r="3">
+      <x v="2"/>
+    </i>
+    <i t="default" r="2">
+      <x v="1"/>
+    </i>
+    <i t="blank" r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+      <x v="4"/>
+      <x/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="4">
+      <x/>
+    </i>
+    <i t="blank" r="4">
+      <x/>
+    </i>
+    <i t="default" r="3">
+      <x v="4"/>
+    </i>
+    <i t="blank" r="3">
+      <x v="4"/>
+    </i>
+    <i t="default" r="2">
+      <x v="2"/>
+    </i>
+    <i t="blank" r="2">
+      <x v="2"/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i t="blank" r="1">
+      <x/>
+    </i>
+    <i t="default">
+      <x v="5"/>
+    </i>
+    <i t="blank">
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
       <x/>
       <x v="1"/>
-      <x v="2"/>
+      <x v="6"/>
+      <x/>
       <x v="3"/>
     </i>
+    <i t="default" r="4">
+      <x/>
+    </i>
     <i t="blank" r="4">
-      <x v="2"/>
+      <x/>
+    </i>
+    <i t="default" r="3">
+      <x v="6"/>
+    </i>
+    <i t="blank" r="3">
+      <x v="6"/>
+    </i>
+    <i t="default" r="2">
+      <x v="1"/>
+    </i>
+    <i t="blank" r="2">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i t="blank" r="1">
+      <x/>
+    </i>
+    <i t="default">
+      <x v="6"/>
+    </i>
+    <i t="blank">
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="8"/>
+      <x/>
+      <x v="1"/>
+      <x v="7"/>
+      <x/>
+      <x v="3"/>
+    </i>
+    <i t="default" r="4">
+      <x/>
+    </i>
+    <i t="blank" r="4">
+      <x/>
+    </i>
+    <i t="default" r="3">
+      <x v="7"/>
+    </i>
+    <i t="blank" r="3">
+      <x v="7"/>
+    </i>
+    <i t="default" r="2">
+      <x v="1"/>
+    </i>
+    <i t="blank" r="2">
+      <x v="1"/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i t="blank" r="1">
+      <x/>
+    </i>
+    <i t="default">
+      <x v="8"/>
+    </i>
+    <i t="blank">
+      <x v="8"/>
     </i>
     <i t="grand">
       <x/>
@@ -3244,10 +3612,7 @@
   <colItems count="1">
     <i/>
   </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of PAID AMOUNT" fld="1" baseField="0" baseItem="7" numFmtId="178"/>
-  </dataFields>
-  <formats count="59">
+  <formats count="43">
     <format dxfId="0">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
@@ -3255,7 +3620,7 @@
       <pivotArea dataOnly="0" labelOnly="1" offset="IV1:IV1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
-            <x v="7"/>
+            <x v="9"/>
           </reference>
         </references>
       </pivotArea>
@@ -3267,7 +3632,7 @@
             <x v="0"/>
           </reference>
           <reference field="0" count="1" selected="0">
-            <x v="7"/>
+            <x v="9"/>
           </reference>
         </references>
       </pivotArea>
@@ -3378,270 +3743,18 @@
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
     <format dxfId="38">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="4">
-          <reference field="3" count="1">
-            <x v="1"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" offset="D1:D1" fieldPosition="0"/>
     </format>
     <format dxfId="39">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="4">
-          <reference field="3" count="1">
-            <x v="2"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="10"/>
-          </reference>
-        </references>
-      </pivotArea>
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
     <format dxfId="40">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="4">
-          <reference field="3" count="1">
-            <x v="1"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="10"/>
-          </reference>
-        </references>
-      </pivotArea>
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" offset="B1:B1" fieldPosition="0"/>
     </format>
     <format dxfId="41">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="4">
-          <reference field="3" count="1">
-            <x v="1"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="11"/>
-          </reference>
-        </references>
-      </pivotArea>
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
     <format dxfId="42">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="4">
-          <reference field="3" count="1">
-            <x v="4"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="12"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="43">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" offset="D1:D1" fieldPosition="0"/>
-    </format>
-    <format dxfId="44">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="4">
-          <reference field="3" count="1">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="45">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="4">
-          <reference field="3" count="1">
-            <x v="2"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="10"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="46">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="4">
-          <reference field="3" count="1">
-            <x v="1"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="10"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="47">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="4">
-          <reference field="3" count="1">
-            <x v="1"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="11"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="48">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="4">
-          <reference field="3" count="1">
-            <x v="4"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="12"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="49">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="50">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="51">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1">
-            <x v="1"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="52">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" offset="B1:B1" fieldPosition="0"/>
-    </format>
-    <format dxfId="53">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="54">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="55">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="56">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="57">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="1" count="1">
-            <x v="3"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="12"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="58">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" offset="B1:B1" fieldPosition="0"/>
     </format>
   </formats>
@@ -3660,25 +3773,31 @@
     <pivotTable tabId="12" name="PivotTable6"/>
   </pivotTables>
   <data>
-    <tabular pivotCacheId="1">
-      <items count="13">
+    <tabular pivotCacheId="1" showMissing="0">
+      <items count="15">
+        <i x="4" s="1"/>
+        <i x="5" s="1"/>
+        <i x="2" s="1"/>
         <i x="0" s="1"/>
-        <i x="3" s="1" nd="1"/>
-        <i x="2" s="1" nd="1"/>
-        <i x="4" s="1" nd="1"/>
-        <i x="6" s="1" nd="1"/>
-        <i x="5" s="1" nd="1"/>
-        <i x="9" s="1" nd="1"/>
+        <i x="1" s="1"/>
+        <i x="3" s="1"/>
+        <i x="6" s="0"/>
         <i x="7" s="1" nd="1"/>
         <i x="8" s="1" nd="1"/>
+        <i x="11" s="1" nd="1"/>
+        <i x="9" s="1" nd="1"/>
         <i x="10" s="1" nd="1"/>
-        <i x="11" s="1" nd="1"/>
         <i x="12" s="1" nd="1"/>
-        <i x="1" s="0" nd="1"/>
+        <i x="13" s="1" nd="1"/>
+        <i x="14" s="1" nd="1"/>
       </items>
     </tabular>
   </data>
-  <extLst/>
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{470722E0-AACD-4C17-9CDC-17EF765DBC7E}">
+      <x15:slicerCacheHideItemsWithNoData/>
+    </x:ext>
+  </extLst>
 </slicerCacheDefinition>
 </file>
 
@@ -3691,14 +3810,18 @@
     <tabular pivotCacheId="1">
       <items count="5">
         <i x="0" s="1"/>
+        <i x="1" s="1"/>
         <i x="4" s="1" nd="1"/>
+        <i x="3" s="1" nd="1"/>
         <i x="2" s="1" nd="1"/>
-        <i x="3" s="1" nd="1"/>
-        <i x="1" s="0" nd="1"/>
       </items>
     </tabular>
   </data>
-  <extLst/>
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{470722E0-AACD-4C17-9CDC-17EF765DBC7E}">
+      <x15:slicerCacheHideItemsWithNoData/>
+    </x:ext>
+  </extLst>
 </slicerCacheDefinition>
 </file>
 
@@ -3711,11 +3834,15 @@
     <tabular pivotCacheId="1">
       <items count="2">
         <i x="0" s="1"/>
-        <i x="1" s="0" nd="1"/>
+        <i x="1" s="1" nd="1"/>
       </items>
     </tabular>
   </data>
-  <extLst/>
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{470722E0-AACD-4C17-9CDC-17EF765DBC7E}">
+      <x15:slicerCacheHideItemsWithNoData/>
+    </x:ext>
+  </extLst>
 </slicerCacheDefinition>
 </file>
 
@@ -3731,12 +3858,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="F3:K1353" totalsRowShown="0">
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="F3:K1353" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="MEMBERS" dataDxfId="59"/>
-    <tableColumn id="2" name="PAID AMOUNT" dataDxfId="60"/>
+    <tableColumn id="1" name="MEMBERS" dataDxfId="43"/>
+    <tableColumn id="2" name="PAID AMOUNT" dataDxfId="44"/>
     <tableColumn id="6" name="Year"/>
     <tableColumn id="5" name="Month"/>
-    <tableColumn id="3" name="Day" dataDxfId="61"/>
-    <tableColumn id="4" name="MODE OF PAYMENT" dataDxfId="62"/>
+    <tableColumn id="3" name="Day" dataDxfId="45"/>
+    <tableColumn id="4" name="MODE OF PAYMENT" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4002,8 +4129,8 @@
   <sheetPr/>
   <dimension ref="A1:S1353"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="21" customHeight="1"/>
@@ -4138,12 +4265,24 @@
       <c r="E5">
         <v>2</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="20"/>
+      <c r="F5" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="20">
+        <v>100</v>
+      </c>
+      <c r="H5" s="19">
+        <v>2025</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="30">
+        <v>21</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>12</v>
+      </c>
       <c r="M5"/>
       <c r="N5"/>
       <c r="O5"/>
@@ -4154,7 +4293,7 @@
     </row>
     <row r="6" customHeight="1" spans="1:19">
       <c r="A6" s="18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="18" t="s">
@@ -4166,12 +4305,24 @@
       <c r="E6">
         <v>3</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="20"/>
+      <c r="F6" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="20">
+        <v>100</v>
+      </c>
+      <c r="H6" s="19">
+        <v>2025</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="30">
+        <v>22</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>12</v>
+      </c>
       <c r="M6"/>
       <c r="N6"/>
       <c r="O6"/>
@@ -4182,11 +4333,11 @@
     </row>
     <row r="7" customHeight="1" spans="1:19">
       <c r="A7" s="18" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="18" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D7" s="18">
         <v>4</v>
@@ -4194,12 +4345,24 @@
       <c r="E7">
         <v>4</v>
       </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="20"/>
+      <c r="F7" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="20">
+        <v>100</v>
+      </c>
+      <c r="H7" s="19">
+        <v>2025</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="30">
+        <v>22</v>
+      </c>
+      <c r="K7" s="20" t="s">
+        <v>12</v>
+      </c>
       <c r="M7"/>
       <c r="N7"/>
       <c r="O7"/>
@@ -4210,11 +4373,11 @@
     </row>
     <row r="8" customHeight="1" spans="1:19">
       <c r="A8" s="18" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="18" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D8" s="18">
         <v>5</v>
@@ -4222,12 +4385,24 @@
       <c r="E8">
         <v>5</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="20"/>
+      <c r="F8" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="20">
+        <v>100</v>
+      </c>
+      <c r="H8" s="19">
+        <v>2025</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="30">
+        <v>23</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>12</v>
+      </c>
       <c r="M8"/>
       <c r="N8"/>
       <c r="O8"/>
@@ -4238,11 +4413,11 @@
     </row>
     <row r="9" customHeight="1" spans="1:19">
       <c r="A9" s="18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D9" s="18">
         <v>6</v>
@@ -4250,12 +4425,24 @@
       <c r="E9">
         <v>6</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="20"/>
+      <c r="F9" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="20">
+        <v>100</v>
+      </c>
+      <c r="H9" s="19">
+        <v>2025</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="30">
+        <v>21</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>12</v>
+      </c>
       <c r="M9"/>
       <c r="N9"/>
       <c r="O9"/>
@@ -4266,11 +4453,11 @@
     </row>
     <row r="10" customHeight="1" spans="1:19">
       <c r="A10" s="18" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B10" s="18"/>
       <c r="C10" s="18" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D10" s="18">
         <v>7</v>
@@ -4278,12 +4465,24 @@
       <c r="E10">
         <v>7</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="20"/>
+      <c r="F10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="20">
+        <v>100</v>
+      </c>
+      <c r="H10" s="19">
+        <v>2025</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="28">
+        <v>19</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>12</v>
+      </c>
       <c r="M10"/>
       <c r="N10"/>
       <c r="O10"/>
@@ -4294,11 +4493,11 @@
     </row>
     <row r="11" customHeight="1" spans="1:19">
       <c r="A11" s="18" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D11" s="18">
         <v>8</v>
@@ -4306,12 +4505,24 @@
       <c r="E11">
         <v>8</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="20"/>
+      <c r="F11" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="20">
+        <v>100</v>
+      </c>
+      <c r="H11" s="19">
+        <v>2025</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="28">
+        <v>26</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>12</v>
+      </c>
       <c r="M11"/>
       <c r="N11"/>
       <c r="O11"/>
@@ -4322,11 +4533,11 @@
     </row>
     <row r="12" customHeight="1" spans="1:19">
       <c r="A12" s="18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D12" s="18">
         <v>9</v>
@@ -4334,12 +4545,24 @@
       <c r="E12">
         <v>9</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="20"/>
+      <c r="F12" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="20">
+        <v>100</v>
+      </c>
+      <c r="H12" s="19">
+        <v>2025</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="28">
+        <v>28</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>12</v>
+      </c>
       <c r="M12"/>
       <c r="N12"/>
       <c r="O12"/>
@@ -4350,11 +4573,11 @@
     </row>
     <row r="13" customHeight="1" spans="1:19">
       <c r="A13" s="18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D13" s="18">
         <v>10</v>
@@ -4362,12 +4585,24 @@
       <c r="E13">
         <v>10</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="20"/>
+      <c r="F13" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="20">
+        <v>100</v>
+      </c>
+      <c r="H13" s="19">
+        <v>2025</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="28">
+        <v>29</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>12</v>
+      </c>
       <c r="M13"/>
       <c r="N13"/>
       <c r="O13"/>
@@ -4378,11 +4613,11 @@
     </row>
     <row r="14" customHeight="1" spans="1:19">
       <c r="A14" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D14" s="18">
         <v>11</v>
@@ -4406,11 +4641,11 @@
     </row>
     <row r="15" customHeight="1" spans="1:19">
       <c r="A15" s="18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D15" s="18">
         <v>12</v>
@@ -4460,7 +4695,7 @@
     </row>
     <row r="17" customHeight="1" spans="1:19">
       <c r="A17" s="18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -4486,7 +4721,7 @@
     </row>
     <row r="18" customHeight="1" spans="1:19">
       <c r="A18" s="18" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
@@ -4512,7 +4747,7 @@
     </row>
     <row r="19" customHeight="1" spans="1:19">
       <c r="A19" s="18" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
@@ -4538,7 +4773,7 @@
     </row>
     <row r="20" customHeight="1" spans="1:19">
       <c r="A20" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
@@ -4564,7 +4799,7 @@
     </row>
     <row r="21" customHeight="1" spans="1:19">
       <c r="A21" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
@@ -4590,7 +4825,7 @@
     </row>
     <row r="22" customHeight="1" spans="1:19">
       <c r="A22" s="18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
@@ -4616,7 +4851,7 @@
     </row>
     <row r="23" customHeight="1" spans="1:19">
       <c r="A23" s="18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
@@ -4642,7 +4877,7 @@
     </row>
     <row r="24" customHeight="1" spans="1:19">
       <c r="A24" s="18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
@@ -4668,7 +4903,7 @@
     </row>
     <row r="25" customHeight="1" spans="1:19">
       <c r="A25" s="18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
@@ -4694,7 +4929,7 @@
     </row>
     <row r="26" customHeight="1" spans="1:11">
       <c r="A26" s="18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
@@ -4713,7 +4948,7 @@
     </row>
     <row r="27" customHeight="1" spans="1:11">
       <c r="A27" s="18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
@@ -4732,7 +4967,7 @@
     </row>
     <row r="28" customHeight="1" spans="1:11">
       <c r="A28" s="18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
@@ -4751,7 +4986,7 @@
     </row>
     <row r="29" customHeight="1" spans="1:11">
       <c r="A29" s="18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
@@ -4770,7 +5005,7 @@
     </row>
     <row r="30" customHeight="1" spans="1:11">
       <c r="A30" s="18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
@@ -4789,7 +5024,7 @@
     </row>
     <row r="31" customHeight="1" spans="1:11">
       <c r="A31" s="18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
@@ -4808,7 +5043,7 @@
     </row>
     <row r="32" customHeight="1" spans="1:11">
       <c r="A32" s="18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
@@ -4827,7 +5062,7 @@
     </row>
     <row r="33" customHeight="1" spans="1:11">
       <c r="A33" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
@@ -4846,7 +5081,7 @@
     </row>
     <row r="34" customHeight="1" spans="1:11">
       <c r="A34" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
@@ -4865,7 +5100,7 @@
     </row>
     <row r="35" customHeight="1" spans="1:11">
       <c r="A35" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E35">
         <v>32</v>
@@ -4879,7 +5114,7 @@
     </row>
     <row r="36" customHeight="1" spans="1:11">
       <c r="A36" s="18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E36">
         <v>33</v>
@@ -4893,7 +5128,7 @@
     </row>
     <row r="37" customHeight="1" spans="1:11">
       <c r="A37" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E37">
         <v>34</v>
@@ -4907,7 +5142,7 @@
     </row>
     <row r="38" customHeight="1" spans="1:11">
       <c r="A38" s="18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E38">
         <v>35</v>
@@ -4921,7 +5156,7 @@
     </row>
     <row r="39" customHeight="1" spans="1:11">
       <c r="A39" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E39">
         <v>36</v>
@@ -4935,7 +5170,7 @@
     </row>
     <row r="40" customHeight="1" spans="1:11">
       <c r="A40" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E40">
         <v>37</v>
@@ -4949,7 +5184,7 @@
     </row>
     <row r="41" customHeight="1" spans="1:11">
       <c r="A41" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E41">
         <v>38</v>
@@ -4963,7 +5198,7 @@
     </row>
     <row r="42" customHeight="1" spans="1:11">
       <c r="A42" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E42">
         <v>39</v>
@@ -19401,18 +19636,18 @@
     <mergeCell ref="F1:K2"/>
   </mergeCells>
   <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H12 H13 H4:H11 H14:H1353">
+      <formula1>$B$4:$B$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I12 I13 I4:I11 I14:I1353">
+      <formula1>$C$4:$C$15</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J12 J13 J4:J11 J14:J1353">
+      <formula1>$D$4:$D$34</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G13 G4:G12 G14:G1353"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F1353">
       <formula1>$A$4:$A$84</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G1353"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H1353">
-      <formula1>$B$4:$B$5</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I1353">
-      <formula1>$C$4:$C$15</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J4:J1353">
-      <formula1>$D$4:$D$34</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -19426,20 +19661,19 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="29.037037037037" customWidth="1"/>
+    <col min="1" max="1" width="25.1111111111111"/>
     <col min="2" max="2" width="21.1111111111111" style="1"/>
     <col min="3" max="3" width="10.4444444444444" customWidth="1"/>
     <col min="4" max="4" width="11.1111111111111" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.77777777777778"/>
-    <col min="6" max="6" width="23.1111111111111"/>
+    <col min="5" max="6" width="23.1111111111111"/>
     <col min="7" max="7" width="21.1111111111111"/>
     <col min="8" max="8" width="4.66666666666667"/>
   </cols>
@@ -19450,263 +19684,975 @@
     <row r="2" spans="4:4">
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="6" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B4" s="6">
+        <v>2025</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="6">
+        <v>23</v>
+      </c>
+      <c r="E4" s="6">
         <v>100</v>
-      </c>
-      <c r="C4" s="6">
-        <v>2025</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="6">
-        <v>3</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="E5" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="F5" s="6"/>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="7"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="8"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="7">
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="6">
+        <v>29</v>
+      </c>
+      <c r="E11" s="6">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9"/>
-      <c r="D9"/>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10"/>
-      <c r="D10"/>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11"/>
-      <c r="D11"/>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12"/>
-      <c r="D12"/>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13"/>
-      <c r="D13"/>
-    </row>
-    <row r="14" spans="2:4">
-      <c r="B14"/>
-      <c r="D14"/>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15"/>
-      <c r="D15"/>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16"/>
-      <c r="D16"/>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17"/>
-      <c r="D17"/>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18"/>
-      <c r="D18"/>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19"/>
-      <c r="D19"/>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20"/>
-      <c r="D20"/>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21"/>
-      <c r="D21"/>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22"/>
-      <c r="D22"/>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23"/>
-      <c r="D23"/>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24"/>
-      <c r="D24"/>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="B25"/>
-      <c r="D25"/>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26"/>
-      <c r="D26"/>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="B27"/>
-      <c r="D27"/>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28"/>
-      <c r="D28"/>
-    </row>
-    <row r="29" spans="2:4">
-      <c r="B29"/>
-      <c r="D29"/>
-    </row>
-    <row r="30" spans="2:4">
-      <c r="B30"/>
-      <c r="D30"/>
-    </row>
-    <row r="31" spans="2:4">
-      <c r="B31"/>
-      <c r="D31"/>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="B32"/>
-      <c r="D32"/>
-    </row>
-    <row r="33" spans="2:4">
-      <c r="B33"/>
-      <c r="D33"/>
-    </row>
-    <row r="34" spans="2:4">
-      <c r="B34"/>
-      <c r="D34"/>
-    </row>
-    <row r="35" spans="2:4">
-      <c r="B35"/>
-      <c r="D35"/>
-    </row>
-    <row r="36" spans="2:4">
-      <c r="B36"/>
-      <c r="D36"/>
-    </row>
-    <row r="37" spans="2:4">
-      <c r="B37"/>
-      <c r="D37"/>
-    </row>
-    <row r="38" spans="2:4">
-      <c r="B38"/>
-      <c r="D38"/>
-    </row>
-    <row r="39" spans="2:4">
-      <c r="B39"/>
-      <c r="D39"/>
-    </row>
-    <row r="40" spans="2:4">
-      <c r="B40"/>
-      <c r="D40"/>
-    </row>
-    <row r="41" spans="2:4">
-      <c r="B41"/>
-      <c r="D41"/>
-    </row>
-    <row r="42" spans="2:4">
-      <c r="B42"/>
-      <c r="D42"/>
-    </row>
-    <row r="43" spans="2:4">
-      <c r="B43"/>
-      <c r="D43"/>
-    </row>
-    <row r="44" spans="2:4">
-      <c r="B44"/>
-      <c r="D44"/>
-    </row>
-    <row r="45" spans="2:4">
-      <c r="B45"/>
-      <c r="D45"/>
-    </row>
-    <row r="46" spans="2:4">
-      <c r="B46"/>
-      <c r="D46"/>
-    </row>
-    <row r="47" spans="2:4">
-      <c r="B47"/>
-      <c r="D47"/>
-    </row>
-    <row r="48" spans="2:4">
-      <c r="B48"/>
-      <c r="D48"/>
-    </row>
-    <row r="49" spans="2:4">
-      <c r="B49"/>
-      <c r="D49"/>
-    </row>
-    <row r="50" spans="2:4">
-      <c r="B50"/>
-      <c r="D50"/>
-    </row>
-    <row r="51" spans="2:4">
-      <c r="B51"/>
-      <c r="D51"/>
-    </row>
-    <row r="52" spans="2:4">
-      <c r="B52"/>
-      <c r="D52"/>
-    </row>
-    <row r="53" spans="2:4">
-      <c r="B53"/>
-      <c r="D53"/>
+      <c r="F11" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="6">
+        <v>2025</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="6">
+        <v>21</v>
+      </c>
+      <c r="E22" s="6">
+        <v>100</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="6">
+        <v>28</v>
+      </c>
+      <c r="E29" s="6">
+        <v>100</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="6">
+        <v>2025</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="6">
+        <v>22</v>
+      </c>
+      <c r="E40" s="6">
+        <v>100</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="6">
+        <v>26</v>
+      </c>
+      <c r="E47" s="6">
+        <v>100</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F48" s="6"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="6"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="6"/>
+      <c r="B54" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="6"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="6"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" s="6">
+        <v>2025</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="6">
+        <v>3</v>
+      </c>
+      <c r="E58" s="6">
+        <v>100</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="6"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F59" s="6"/>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="6"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="6"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="6"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="6"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="6"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="6"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D65" s="6">
+        <v>19</v>
+      </c>
+      <c r="E65" s="6">
+        <v>100</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="6"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F66" s="6"/>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="6"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="6"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="6"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="6"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="6"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="6"/>
+      <c r="B72" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="6"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="6"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B76" s="6">
+        <v>2025</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D76" s="6">
+        <v>21</v>
+      </c>
+      <c r="E76" s="6">
+        <v>100</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="6"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F77" s="6"/>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="6"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="6"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="6"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="6"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="6"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="6"/>
+      <c r="B83" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="6"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="6"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B87" s="6">
+        <v>2025</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D87" s="6">
+        <v>22</v>
+      </c>
+      <c r="E87" s="6">
+        <v>100</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="6"/>
+      <c r="B88" s="6"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F88" s="6"/>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="6"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="6"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="6"/>
+      <c r="B91" s="6"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="6"/>
+      <c r="B92" s="6"/>
+      <c r="C92" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="6"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="6"/>
+      <c r="B94" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="6"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B96" s="6"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="6"/>
+      <c r="B97" s="6"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B98" s="7"/>
+      <c r="C98" s="6"/>
+      <c r="D98" s="8"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -19727,8 +20673,8 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>

</xml_diff>